<commit_message>
Fixed score calcs, added quartile feature
</commit_message>
<xml_diff>
--- a/CRIq_dataworksheet_m.xlsx
+++ b/CRIq_dataworksheet_m.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\CRIq_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Thesis Work\CRIq_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="221">
   <si>
     <t>Age</t>
   </si>
@@ -558,9 +558,6 @@
   </si>
   <si>
     <t>43.97</t>
-  </si>
-  <si>
-    <t>84.6</t>
   </si>
   <si>
     <t>52.88</t>
@@ -1204,34 +1201,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG162" workbookViewId="0">
-      <selection activeCell="AQ181" sqref="AQ181"/>
+    <sheetView tabSelected="1" topLeftCell="AG34" workbookViewId="0">
+      <selection activeCell="AZ59" sqref="AZ59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="5"/>
-    <col min="3" max="4" width="9.109375" style="6"/>
-    <col min="5" max="9" width="9.109375" style="7"/>
-    <col min="10" max="14" width="9.109375" style="11"/>
-    <col min="15" max="20" width="9.109375" style="16"/>
-    <col min="21" max="23" width="9.109375" style="8"/>
-    <col min="24" max="26" width="9.109375" style="19"/>
-    <col min="27" max="32" width="9.109375" style="12"/>
-    <col min="33" max="36" width="9.109375" style="6"/>
-    <col min="37" max="37" width="9.109375" style="5"/>
-    <col min="38" max="39" width="9.109375" style="16"/>
-    <col min="40" max="41" width="9.109375" style="8"/>
-    <col min="42" max="43" width="9.109375" style="7"/>
-    <col min="44" max="46" width="9.109375" style="19"/>
-    <col min="47" max="47" width="9.109375" style="6"/>
-    <col min="48" max="49" width="9.109375" style="29"/>
-    <col min="50" max="50" width="9.109375" style="31"/>
-    <col min="51" max="51" width="9.109375" style="8"/>
-    <col min="52" max="52" width="9.109375" style="23"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="3" max="4" width="9.140625" style="6"/>
+    <col min="5" max="9" width="9.140625" style="7"/>
+    <col min="10" max="14" width="9.140625" style="11"/>
+    <col min="15" max="20" width="9.140625" style="16"/>
+    <col min="21" max="23" width="9.140625" style="8"/>
+    <col min="24" max="26" width="9.140625" style="19"/>
+    <col min="27" max="32" width="9.140625" style="12"/>
+    <col min="33" max="36" width="9.140625" style="6"/>
+    <col min="37" max="37" width="9.140625" style="5"/>
+    <col min="38" max="39" width="9.140625" style="16"/>
+    <col min="40" max="41" width="9.140625" style="8"/>
+    <col min="42" max="43" width="9.140625" style="7"/>
+    <col min="44" max="46" width="9.140625" style="19"/>
+    <col min="47" max="47" width="9.140625" style="6"/>
+    <col min="48" max="49" width="9.140625" style="29"/>
+    <col min="50" max="50" width="9.140625" style="31"/>
+    <col min="51" max="51" width="9.140625" style="8"/>
+    <col min="52" max="52" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
@@ -1395,7 +1392,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>181</v>
       </c>
@@ -1552,7 +1549,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>182</v>
       </c>
@@ -1699,7 +1696,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>211</v>
       </c>
@@ -1825,7 +1822,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>212</v>
       </c>
@@ -1963,7 +1960,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>213</v>
       </c>
@@ -2110,7 +2107,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>214</v>
       </c>
@@ -2251,7 +2248,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>215</v>
       </c>
@@ -2398,7 +2395,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>216</v>
       </c>
@@ -2545,7 +2542,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>217</v>
       </c>
@@ -2692,7 +2689,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>218</v>
       </c>
@@ -2833,7 +2830,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>241</v>
       </c>
@@ -2980,7 +2977,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>242</v>
       </c>
@@ -3121,7 +3118,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>243</v>
       </c>
@@ -3268,7 +3265,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>244</v>
       </c>
@@ -3415,7 +3412,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>245</v>
       </c>
@@ -3562,7 +3559,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>246</v>
       </c>
@@ -3709,7 +3706,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>247</v>
       </c>
@@ -3856,7 +3853,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>248</v>
       </c>
@@ -4003,7 +4000,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>249</v>
       </c>
@@ -4150,7 +4147,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>250</v>
       </c>
@@ -4297,7 +4294,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>251</v>
       </c>
@@ -4444,7 +4441,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>253</v>
       </c>
@@ -4591,7 +4588,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>254</v>
       </c>
@@ -4738,7 +4735,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>255</v>
       </c>
@@ -4885,7 +4882,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>256</v>
       </c>
@@ -5032,7 +5029,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>257</v>
       </c>
@@ -5179,7 +5176,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>258</v>
       </c>
@@ -5326,7 +5323,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>61</v>
       </c>
@@ -5473,7 +5470,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>62</v>
       </c>
@@ -5620,7 +5617,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>63</v>
       </c>
@@ -5767,7 +5764,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>64</v>
       </c>
@@ -5914,7 +5911,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>65</v>
       </c>
@@ -6061,7 +6058,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>66</v>
       </c>
@@ -6208,7 +6205,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>67</v>
       </c>
@@ -6355,7 +6352,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>68</v>
       </c>
@@ -6502,7 +6499,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>69</v>
       </c>
@@ -6649,7 +6646,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>70</v>
       </c>
@@ -6796,7 +6793,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>71</v>
       </c>
@@ -6943,7 +6940,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>72</v>
       </c>
@@ -7090,7 +7087,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>91</v>
       </c>
@@ -7237,7 +7234,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>92</v>
       </c>
@@ -7384,7 +7381,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>93</v>
       </c>
@@ -7531,7 +7528,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>94</v>
       </c>
@@ -7678,7 +7675,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>95</v>
       </c>
@@ -7825,7 +7822,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>96</v>
       </c>
@@ -7972,7 +7969,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>97</v>
       </c>
@@ -8119,7 +8116,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>98</v>
       </c>
@@ -8266,7 +8263,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>99</v>
       </c>
@@ -8413,7 +8410,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>421</v>
       </c>
@@ -8521,7 +8518,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="51" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>422</v>
       </c>
@@ -8629,7 +8626,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>423</v>
       </c>
@@ -8737,7 +8734,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>424</v>
       </c>
@@ -8845,7 +8842,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="54" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>425</v>
       </c>
@@ -8953,7 +8950,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="55" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>426</v>
       </c>
@@ -9061,7 +9058,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="56" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>427</v>
       </c>
@@ -9169,7 +9166,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>1</v>
       </c>
@@ -9316,7 +9313,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>2</v>
       </c>
@@ -9463,7 +9460,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>3</v>
       </c>
@@ -9606,11 +9603,11 @@
       <c r="AY59" s="8">
         <v>26</v>
       </c>
-      <c r="AZ59" s="23" t="s">
-        <v>179</v>
+      <c r="AZ59" s="23">
+        <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>5</v>
       </c>
@@ -9757,7 +9754,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>6</v>
       </c>
@@ -9904,7 +9901,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>31</v>
       </c>
@@ -10018,10 +10015,10 @@
         <v>11</v>
       </c>
       <c r="AN62" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="AO62" s="8" t="s">
         <v>183</v>
-      </c>
-      <c r="AO62" s="8" t="s">
-        <v>184</v>
       </c>
       <c r="AP62" s="7">
         <v>8</v>
@@ -10030,13 +10027,13 @@
         <v>8</v>
       </c>
       <c r="AR62" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="AS62" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="AS62" s="19" t="s">
+      <c r="AT62" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="AT62" s="19" t="s">
-        <v>182</v>
       </c>
       <c r="AU62" s="6">
         <v>45</v>
@@ -10051,7 +10048,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="63" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>32</v>
       </c>
@@ -10162,7 +10159,7 @@
         <v>11</v>
       </c>
       <c r="AM63" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AU63" s="6">
         <v>21</v>
@@ -10177,7 +10174,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>33</v>
       </c>
@@ -10291,10 +10288,10 @@
         <v>66</v>
       </c>
       <c r="AN64" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="AO64" s="8" t="s">
         <v>186</v>
-      </c>
-      <c r="AO64" s="8" t="s">
-        <v>187</v>
       </c>
       <c r="AP64" s="7">
         <v>9</v>
@@ -10303,13 +10300,13 @@
         <v>9</v>
       </c>
       <c r="AR64" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="AS64" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="AS64" s="19" t="s">
+      <c r="AT64" s="19" t="s">
         <v>189</v>
-      </c>
-      <c r="AT64" s="19" t="s">
-        <v>190</v>
       </c>
       <c r="AU64" s="6">
         <v>42</v>
@@ -10324,7 +10321,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>34</v>
       </c>
@@ -10432,16 +10429,16 @@
         <v>34</v>
       </c>
       <c r="AL65" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AM65" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AN65" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="AO65" s="8" t="s">
         <v>195</v>
-      </c>
-      <c r="AO65" s="8" t="s">
-        <v>196</v>
       </c>
       <c r="AP65" s="7">
         <v>8</v>
@@ -10450,13 +10447,13 @@
         <v>5</v>
       </c>
       <c r="AR65" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="AS65" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="AS65" s="19" t="s">
+      <c r="AT65" s="19" t="s">
         <v>193</v>
-      </c>
-      <c r="AT65" s="19" t="s">
-        <v>194</v>
       </c>
       <c r="AU65" s="6">
         <v>37</v>
@@ -10471,7 +10468,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="66" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>35</v>
       </c>
@@ -10582,13 +10579,13 @@
         <v>16</v>
       </c>
       <c r="AM66" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AN66" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="AO66" s="8" t="s">
         <v>197</v>
-      </c>
-      <c r="AO66" s="8" t="s">
-        <v>198</v>
       </c>
       <c r="AP66" s="7">
         <v>9</v>
@@ -10597,13 +10594,13 @@
         <v>9</v>
       </c>
       <c r="AR66" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="AS66" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="AS66" s="19" t="s">
+      <c r="AT66" s="19" t="s">
         <v>200</v>
-      </c>
-      <c r="AT66" s="19" t="s">
-        <v>201</v>
       </c>
       <c r="AU66" s="6">
         <v>37</v>
@@ -10618,7 +10615,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>36</v>
       </c>
@@ -10732,10 +10729,10 @@
         <v>6</v>
       </c>
       <c r="AN67" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="AO67" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="AO67" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="AP67" s="7">
         <v>8</v>
@@ -10744,13 +10741,13 @@
         <v>6</v>
       </c>
       <c r="AR67" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="AS67" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="AS67" s="19" t="s">
+      <c r="AT67" s="19" t="s">
         <v>203</v>
-      </c>
-      <c r="AT67" s="19" t="s">
-        <v>204</v>
       </c>
       <c r="AU67" s="6">
         <v>40</v>
@@ -10765,7 +10762,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>37</v>
       </c>
@@ -10879,10 +10876,10 @@
         <v>68</v>
       </c>
       <c r="AN68" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="AO68" s="8" t="s">
         <v>210</v>
-      </c>
-      <c r="AO68" s="8" t="s">
-        <v>211</v>
       </c>
       <c r="AP68" s="7">
         <v>3.3</v>
@@ -10891,13 +10888,13 @@
         <v>4.2</v>
       </c>
       <c r="AR68" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="AS68" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="AS68" s="19" t="s">
+      <c r="AT68" s="19" t="s">
         <v>208</v>
-      </c>
-      <c r="AT68" s="19" t="s">
-        <v>209</v>
       </c>
       <c r="AU68" s="6">
         <v>39</v>
@@ -10912,7 +10909,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>73</v>
       </c>
@@ -11059,7 +11056,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>331</v>
       </c>
@@ -11167,7 +11164,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="71" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>302</v>
       </c>
@@ -11275,7 +11272,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="72" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>303</v>
       </c>
@@ -11383,7 +11380,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="73" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>364</v>
       </c>
@@ -11491,7 +11488,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="74" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>365</v>
       </c>
@@ -11599,7 +11596,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="75" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>366</v>
       </c>
@@ -11707,7 +11704,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="76" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>367</v>
       </c>
@@ -11815,7 +11812,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="77" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>368</v>
       </c>
@@ -11923,7 +11920,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="78" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>369</v>
       </c>
@@ -12031,7 +12028,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="79" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>370</v>
       </c>
@@ -12139,7 +12136,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="80" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>371</v>
       </c>
@@ -12247,7 +12244,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="81" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>372</v>
       </c>
@@ -12355,7 +12352,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="82" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>373</v>
       </c>
@@ -12463,7 +12460,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="83" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>374</v>
       </c>
@@ -12571,7 +12568,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="84" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>375</v>
       </c>
@@ -12679,7 +12676,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="85" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>376</v>
       </c>
@@ -12787,7 +12784,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="86" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>377</v>
       </c>
@@ -12895,7 +12892,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="87" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>378</v>
       </c>
@@ -13003,7 +13000,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="88" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>379</v>
       </c>
@@ -13111,7 +13108,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="89" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>271</v>
       </c>
@@ -13258,7 +13255,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>272</v>
       </c>
@@ -13405,7 +13402,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>273</v>
       </c>
@@ -13549,7 +13546,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>274</v>
       </c>
@@ -13693,7 +13690,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>275</v>
       </c>
@@ -13837,7 +13834,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>276</v>
       </c>
@@ -13981,7 +13978,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>277</v>
       </c>
@@ -14125,7 +14122,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="96" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>278</v>
       </c>
@@ -14269,7 +14266,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="97" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>279</v>
       </c>
@@ -14413,7 +14410,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="98" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>301</v>
       </c>
@@ -14557,7 +14554,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="99" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>302</v>
       </c>
@@ -14701,7 +14698,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="100" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>303</v>
       </c>
@@ -14845,7 +14842,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>304</v>
       </c>
@@ -14989,7 +14986,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="102" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>305</v>
       </c>
@@ -15133,7 +15130,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="103" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>306</v>
       </c>
@@ -15277,7 +15274,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="104" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>307</v>
       </c>
@@ -15421,7 +15418,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="105" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>308</v>
       </c>
@@ -15565,7 +15562,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>309</v>
       </c>
@@ -15709,7 +15706,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>310</v>
       </c>
@@ -15853,7 +15850,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="108" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>332</v>
       </c>
@@ -16000,7 +15997,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="109" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>333</v>
       </c>
@@ -16147,7 +16144,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="110" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>334</v>
       </c>
@@ -16294,7 +16291,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="111" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>335</v>
       </c>
@@ -16441,7 +16438,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="112" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>336</v>
       </c>
@@ -16588,7 +16585,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="113" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>337</v>
       </c>
@@ -16735,7 +16732,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="114" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>338</v>
       </c>
@@ -16882,7 +16879,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>339</v>
       </c>
@@ -17017,7 +17014,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="116" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>340</v>
       </c>
@@ -17164,7 +17161,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="117" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
         <v>533</v>
       </c>
@@ -17311,7 +17308,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>534</v>
       </c>
@@ -17458,7 +17455,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="119" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>535</v>
       </c>
@@ -17605,7 +17602,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="120" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>428</v>
       </c>
@@ -17752,7 +17749,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="121" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>429</v>
       </c>
@@ -17899,7 +17896,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="122" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>430</v>
       </c>
@@ -18046,7 +18043,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="123" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>403</v>
       </c>
@@ -18193,7 +18190,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="124" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>402</v>
       </c>
@@ -18340,7 +18337,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="125" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>401</v>
       </c>
@@ -18487,7 +18484,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="126" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>400</v>
       </c>
@@ -18634,7 +18631,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="127" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>399</v>
       </c>
@@ -18781,7 +18778,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="128" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>398</v>
       </c>
@@ -18928,7 +18925,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="129" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>391</v>
       </c>
@@ -19075,7 +19072,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="130" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>397</v>
       </c>
@@ -19222,7 +19219,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="131" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
         <v>396</v>
       </c>
@@ -19326,7 +19323,7 @@
         <v>137</v>
       </c>
       <c r="AK131" s="5">
-        <f t="shared" ref="AK131:AK194" si="11">A131</f>
+        <f t="shared" ref="AK131:AK189" si="11">A131</f>
         <v>396</v>
       </c>
       <c r="AL131" s="16">
@@ -19369,7 +19366,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="132" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
         <v>395</v>
       </c>
@@ -19516,7 +19513,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="133" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A133" s="5">
         <v>394</v>
       </c>
@@ -19663,7 +19660,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="134" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A134" s="5">
         <v>393</v>
       </c>
@@ -19810,7 +19807,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="135" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A135" s="5">
         <v>392</v>
       </c>
@@ -19957,7 +19954,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="136" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
         <v>526</v>
       </c>
@@ -20104,7 +20101,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="137" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A137" s="5">
         <v>539</v>
       </c>
@@ -20251,7 +20248,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="138" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A138" s="5">
         <v>540</v>
       </c>
@@ -20398,7 +20395,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="139" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A139" s="5">
         <v>542</v>
       </c>
@@ -20545,7 +20542,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="140" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A140" s="5">
         <v>545</v>
       </c>
@@ -20692,7 +20689,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="141" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A141" s="5">
         <v>548</v>
       </c>
@@ -20839,7 +20836,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="142" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A142" s="5">
         <v>560</v>
       </c>
@@ -20986,7 +20983,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="143" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A143" s="5">
         <v>570</v>
       </c>
@@ -21124,16 +21121,16 @@
         <v>34</v>
       </c>
       <c r="AX143" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AY143" s="8">
         <v>29</v>
       </c>
       <c r="AZ143" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
-    <row r="144" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
         <v>571</v>
       </c>
@@ -21280,7 +21277,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="145" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A145" s="5">
         <v>573</v>
       </c>
@@ -21427,7 +21424,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="146" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A146" s="5">
         <v>575</v>
       </c>
@@ -21574,7 +21571,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="147" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A147" s="5">
         <v>451</v>
       </c>
@@ -21721,7 +21718,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="148" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A148" s="5">
         <v>452</v>
       </c>
@@ -21868,7 +21865,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="149" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A149" s="5">
         <v>453</v>
       </c>
@@ -22015,7 +22012,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="150" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A150" s="5">
         <v>454</v>
       </c>
@@ -22162,7 +22159,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="151" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A151" s="5">
         <v>455</v>
       </c>
@@ -22309,7 +22306,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="152" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
         <v>456</v>
       </c>
@@ -22456,7 +22453,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="153" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A153" s="5">
         <v>457</v>
       </c>
@@ -22603,7 +22600,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="154" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A154" s="5">
         <v>458</v>
       </c>
@@ -22750,7 +22747,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="155" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A155" s="5">
         <v>459</v>
       </c>
@@ -22897,7 +22894,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="156" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A156" s="5">
         <v>460</v>
       </c>
@@ -23044,7 +23041,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="157" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A157" s="5">
         <v>461</v>
       </c>
@@ -23191,7 +23188,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="158" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A158" s="5">
         <v>462</v>
       </c>
@@ -23338,7 +23335,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="159" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A159" s="5">
         <v>481</v>
       </c>
@@ -23485,7 +23482,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="160" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A160" s="5">
         <v>121</v>
       </c>
@@ -23632,7 +23629,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="161" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A161" s="5">
         <v>122</v>
       </c>
@@ -23779,7 +23776,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="162" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A162" s="5">
         <v>123</v>
       </c>
@@ -23926,7 +23923,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="163" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A163" s="5">
         <v>124</v>
       </c>
@@ -24073,7 +24070,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="164" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A164" s="5">
         <v>125</v>
       </c>
@@ -24220,7 +24217,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="165" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A165" s="5">
         <v>151</v>
       </c>
@@ -24367,7 +24364,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="166" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A166" s="5">
         <v>152</v>
       </c>
@@ -24429,7 +24426,7 @@
         <v>15</v>
       </c>
       <c r="U166" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="V166" s="8">
         <v>50</v>
@@ -24441,7 +24438,7 @@
         <v>1</v>
       </c>
       <c r="Y166" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Z166" s="19">
         <v>20</v>
@@ -24514,7 +24511,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="167" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A167" s="5">
         <v>153</v>
       </c>
@@ -24564,7 +24561,7 @@
         <v>0</v>
       </c>
       <c r="Q167" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="R167" s="16" t="s">
         <v>31</v>
@@ -24661,7 +24658,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="168" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A168" s="5">
         <v>100</v>
       </c>
@@ -24808,7 +24805,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="169" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A169" s="5">
         <v>101</v>
       </c>
@@ -24955,7 +24952,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="170" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A170" s="5">
         <v>426</v>
       </c>
@@ -25099,7 +25096,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="171" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A171" s="5">
         <v>500</v>
       </c>
@@ -25107,7 +25104,7 @@
         <v>31</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D171" s="6">
         <v>0</v>
@@ -25243,7 +25240,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="172" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A172" s="5">
         <v>520</v>
       </c>
@@ -25278,7 +25275,7 @@
         <v>10</v>
       </c>
       <c r="L172" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M172" s="11">
         <v>0</v>
@@ -25290,7 +25287,7 @@
         <v>15</v>
       </c>
       <c r="P172" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q172" s="16">
         <v>0</v>
@@ -25387,7 +25384,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="173" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A173" s="5">
         <v>521</v>
       </c>
@@ -25531,7 +25528,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="174" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A174" s="5">
         <v>525</v>
       </c>
@@ -25560,10 +25557,10 @@
         <v>0</v>
       </c>
       <c r="J174" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K174" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L174" s="11">
         <v>0</v>
@@ -25675,7 +25672,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="175" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A175" s="5">
         <v>527</v>
       </c>
@@ -25819,7 +25816,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="176" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A176" s="5">
         <v>528</v>
       </c>
@@ -25963,7 +25960,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="177" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A177" s="5">
         <v>530</v>
       </c>
@@ -26031,7 +26028,7 @@
         <v>0</v>
       </c>
       <c r="W177" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X177" s="19">
         <v>0</v>
@@ -26101,13 +26098,13 @@
         <v>46</v>
       </c>
       <c r="AY177" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AZ177" s="23">
         <v>72</v>
       </c>
     </row>
-    <row r="178" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A178" s="5">
         <v>531</v>
       </c>
@@ -26251,7 +26248,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="179" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A179" s="5">
         <v>532</v>
       </c>
@@ -26395,7 +26392,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="180" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A180" s="5">
         <v>536</v>
       </c>
@@ -26539,7 +26536,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="181" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A181" s="5">
         <v>537</v>
       </c>
@@ -26683,7 +26680,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="182" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A182" s="5">
         <v>538</v>
       </c>
@@ -26827,7 +26824,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="183" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A183" s="5">
         <v>543</v>
       </c>
@@ -26959,7 +26956,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="184" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A184" s="5">
         <v>550</v>
       </c>
@@ -27091,7 +27088,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="185" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A185" s="5">
         <v>549</v>
       </c>
@@ -27223,7 +27220,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="186" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A186" s="5">
         <v>551</v>
       </c>
@@ -27352,10 +27349,10 @@
         <v>31</v>
       </c>
       <c r="AZ186" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
-    <row r="187" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A187" s="5">
         <v>552</v>
       </c>
@@ -27487,7 +27484,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="188" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A188" s="5">
         <v>561</v>
       </c>
@@ -27631,7 +27628,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="189" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A189" s="5">
         <v>562</v>
       </c>
@@ -27787,7 +27784,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27799,7 +27796,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>